<commit_message>
Start of data wrangling
may need to find new info
</commit_message>
<xml_diff>
--- a/Data files/Asthma by state.xlsx
+++ b/Data files/Asthma by state.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3A99E0-252D-449C-B121-AFB90E317A6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCAC1FC-0F10-4B40-A5AE-BB1F289AED4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,69 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
-  <si>
-    <t>State or Territory</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Number With Current Asthma</t>
   </si>
   <si>
-    <t>Percent With Current Asthma (SE)</t>
-  </si>
-  <si>
     <t>Alabama</t>
   </si>
   <si>
-    <t>10.1 (0.62)</t>
-  </si>
-  <si>
     <t>Alaska</t>
   </si>
   <si>
-    <t>9.0 (0.58)</t>
-  </si>
-  <si>
     <t>Arizona</t>
   </si>
   <si>
-    <t>9.4 (0.39)</t>
-  </si>
-  <si>
     <t>Arkansas</t>
   </si>
   <si>
-    <t>9.0 (0.62)</t>
-  </si>
-  <si>
     <t>California</t>
   </si>
   <si>
-    <t>8.8 (0.45)</t>
-  </si>
-  <si>
     <t>Colorado</t>
   </si>
   <si>
-    <t>10.4 (0.37)</t>
-  </si>
-  <si>
     <t>Connecticut</t>
   </si>
   <si>
-    <t>10.5 (0.48)</t>
-  </si>
-  <si>
     <t>Delaware</t>
   </si>
   <si>
-    <t>9.8 (0.69)</t>
-  </si>
-  <si>
     <t>District of Columbia</t>
-  </si>
-  <si>
-    <t>11.6 (0.82)</t>
   </si>
   <si>
     <t>Florida</t>
@@ -105,265 +72,139 @@
     <t>Georgia</t>
   </si>
   <si>
-    <t>9.4 (0.51)</t>
-  </si>
-  <si>
     <t>Hawaii</t>
   </si>
   <si>
-    <t>8.1 (0.43)</t>
-  </si>
-  <si>
     <t>Idaho</t>
   </si>
   <si>
-    <t>9.8 (0.46)</t>
-  </si>
-  <si>
     <t>Illinois</t>
   </si>
   <si>
-    <t>8.7 (0.70)</t>
-  </si>
-  <si>
     <t>Indiana</t>
   </si>
   <si>
-    <t>10.3 (0.39)</t>
-  </si>
-  <si>
     <t>Iowa</t>
   </si>
   <si>
-    <t>9.1 (0.41)</t>
-  </si>
-  <si>
     <t>Kansas</t>
   </si>
   <si>
-    <t>10.6 (0.31)</t>
-  </si>
-  <si>
     <t>Kentucky</t>
   </si>
   <si>
-    <t>11.7 (0.59)</t>
-  </si>
-  <si>
     <t>Louisiana</t>
   </si>
   <si>
-    <t>9.7 (0.60)</t>
-  </si>
-  <si>
     <t>Maine</t>
   </si>
   <si>
-    <t>12.5 (0.47)</t>
-  </si>
-  <si>
     <t>Maryland</t>
   </si>
   <si>
-    <t>9.4 (0.35)</t>
-  </si>
-  <si>
     <t>Massachusetts</t>
   </si>
   <si>
-    <t>11.7 (0.52)</t>
-  </si>
-  <si>
     <t>Michigan</t>
   </si>
   <si>
-    <t>11.5 (0.45)</t>
-  </si>
-  <si>
     <t>Minnesota</t>
   </si>
   <si>
-    <t>8.8 (0.28)</t>
-  </si>
-  <si>
     <t>Mississippi</t>
   </si>
   <si>
-    <t>10.0 (0.67)</t>
-  </si>
-  <si>
     <t>Missouri</t>
   </si>
   <si>
-    <t>9.4 (0.42)</t>
-  </si>
-  <si>
     <t>Montana</t>
   </si>
   <si>
-    <t>9.7 (0.48)</t>
-  </si>
-  <si>
     <t>Nebraska</t>
   </si>
   <si>
-    <t>8.2 (0.33)</t>
-  </si>
-  <si>
     <t>Nevada</t>
   </si>
   <si>
-    <t>9.1 (0.80)</t>
-  </si>
-  <si>
     <t>New Hampshire</t>
   </si>
   <si>
-    <t>12.1 (0.60)</t>
-  </si>
-  <si>
     <t>New Jersey</t>
   </si>
   <si>
-    <t>8.9 (0.46)</t>
-  </si>
-  <si>
     <t>New Mexico</t>
   </si>
   <si>
-    <t>10.6 (0.53)</t>
-  </si>
-  <si>
     <t>New York</t>
   </si>
   <si>
-    <t>9.8 (0.28)</t>
-  </si>
-  <si>
     <t>North Carolina</t>
   </si>
   <si>
-    <t>8.7 (0.51)</t>
-  </si>
-  <si>
     <t>North Dakota</t>
   </si>
   <si>
-    <t>8.4 (0.50)</t>
-  </si>
-  <si>
     <t>Ohio</t>
   </si>
   <si>
-    <t>10.4 (0.38)</t>
-  </si>
-  <si>
     <t>Oklahoma</t>
   </si>
   <si>
-    <t>10.9 (0.54)</t>
-  </si>
-  <si>
     <t>Oregon</t>
   </si>
   <si>
-    <t>11.2 (0.53)</t>
-  </si>
-  <si>
     <t>Pennsylvania</t>
   </si>
   <si>
-    <t>10.3 (0.51)</t>
-  </si>
-  <si>
     <t>Rhode Island</t>
   </si>
   <si>
-    <t>12.6 (0.62)</t>
-  </si>
-  <si>
     <t>South Carolina</t>
   </si>
   <si>
-    <t>9.2 (0.45)</t>
-  </si>
-  <si>
     <t>South Dakota</t>
   </si>
   <si>
-    <t>8.3 (0.78)</t>
-  </si>
-  <si>
     <t>Tennessee</t>
   </si>
   <si>
-    <t>10.3 (0.59)</t>
-  </si>
-  <si>
     <t>Texas</t>
   </si>
   <si>
-    <t>8.4 (0.45)</t>
-  </si>
-  <si>
     <t>Utah</t>
   </si>
   <si>
-    <t>9.7 (0.38)</t>
-  </si>
-  <si>
     <t>Vermont</t>
   </si>
   <si>
-    <t>11.8 (0.61)</t>
-  </si>
-  <si>
     <t>Virginia</t>
   </si>
   <si>
-    <t>9.8 (0.41)</t>
-  </si>
-  <si>
     <t>Washington</t>
   </si>
   <si>
-    <t>10.5 (0.36)</t>
-  </si>
-  <si>
     <t>West Virginia</t>
   </si>
   <si>
-    <t>12.1 (0.50)</t>
-  </si>
-  <si>
     <t>Wisconsin</t>
   </si>
   <si>
-    <t>10.8 (0.59)</t>
-  </si>
-  <si>
     <t>Wyoming</t>
   </si>
   <si>
-    <t>9.7 (0.67)</t>
-  </si>
-  <si>
     <t>Guam</t>
   </si>
   <si>
-    <t>4.7 (0.78)</t>
-  </si>
-  <si>
     <t>Puerto Rico</t>
   </si>
   <si>
-    <t>11.4 (0.66)</t>
-  </si>
-  <si>
     <t>Virgin Islands</t>
   </si>
   <si>
-    <t>5.0 (1.02)</t>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Percent With Current Asthma</t>
   </si>
 </sst>
 </file>
@@ -690,7 +531,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -702,607 +543,607 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>394199</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="C2">
+        <v>10.1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>49453</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="C3">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>519749</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="C4">
+        <v>9.4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>207857</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
+      <c r="C5">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2694396</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
+      <c r="C6">
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>476932</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
+      <c r="C7">
+        <v>10.4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>300910</v>
       </c>
-      <c r="C8" t="s">
-        <v>16</v>
+      <c r="C8">
+        <v>10.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>77695</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
+      <c r="C9">
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>64298</v>
       </c>
-      <c r="C10" t="s">
-        <v>20</v>
+      <c r="C10">
+        <v>11.6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>772663</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
+      <c r="C12">
+        <v>9.4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>92849</v>
       </c>
-      <c r="C13" t="s">
-        <v>26</v>
+      <c r="C13">
+        <v>8.1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>138516</v>
       </c>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="C14">
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>860395</v>
       </c>
-      <c r="C15" t="s">
-        <v>30</v>
+      <c r="C15">
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>536397</v>
       </c>
-      <c r="C16" t="s">
-        <v>32</v>
+      <c r="C16">
+        <v>10.3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>224466</v>
       </c>
-      <c r="C17" t="s">
-        <v>34</v>
+      <c r="C17">
+        <v>9.1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>235953</v>
       </c>
-      <c r="C18" t="s">
-        <v>36</v>
+      <c r="C18">
+        <v>10.6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>408801</v>
       </c>
-      <c r="C19" t="s">
-        <v>38</v>
+      <c r="C19">
+        <v>11.7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>344842</v>
       </c>
-      <c r="C20" t="s">
-        <v>40</v>
+      <c r="C20">
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>138396</v>
       </c>
-      <c r="C21" t="s">
-        <v>42</v>
+      <c r="C21">
+        <v>12.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>451158</v>
       </c>
-      <c r="C22" t="s">
-        <v>44</v>
+      <c r="C22">
+        <v>9.4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>661306</v>
       </c>
-      <c r="C23" t="s">
-        <v>46</v>
+      <c r="C23">
+        <v>11.7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>908568</v>
       </c>
-      <c r="C24" t="s">
-        <v>48</v>
+      <c r="C24">
+        <v>11.5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>387219</v>
       </c>
-      <c r="C25" t="s">
-        <v>50</v>
+      <c r="C25">
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>226646</v>
       </c>
-      <c r="C26" t="s">
-        <v>52</v>
+      <c r="C26">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>449253</v>
       </c>
-      <c r="C27" t="s">
-        <v>54</v>
+      <c r="C27">
+        <v>9.4</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>83698</v>
       </c>
-      <c r="C28" t="s">
-        <v>56</v>
+      <c r="C28">
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>122491</v>
       </c>
-      <c r="C29" t="s">
-        <v>58</v>
+      <c r="C29">
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>223954</v>
       </c>
-      <c r="C30" t="s">
-        <v>60</v>
+      <c r="C30">
+        <v>9.1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>136025</v>
       </c>
-      <c r="C31" t="s">
-        <v>62</v>
+      <c r="C31">
+        <v>12.1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>646963</v>
       </c>
-      <c r="C32" t="s">
-        <v>64</v>
+      <c r="C32">
+        <v>8.9</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>173518</v>
       </c>
-      <c r="C33" t="s">
-        <v>66</v>
+      <c r="C33">
+        <v>10.6</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>1563485</v>
       </c>
-      <c r="C34" t="s">
-        <v>68</v>
+      <c r="C34">
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>717344</v>
       </c>
-      <c r="C35" t="s">
-        <v>70</v>
+      <c r="C35">
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>50012</v>
       </c>
-      <c r="C36" t="s">
-        <v>72</v>
+      <c r="C36">
+        <v>8.4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B37">
         <v>955568</v>
       </c>
-      <c r="C37" t="s">
-        <v>74</v>
+      <c r="C37">
+        <v>10.4</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B38">
         <v>326087</v>
       </c>
-      <c r="C38" t="s">
-        <v>76</v>
+      <c r="C38">
+        <v>10.9</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>377851</v>
       </c>
-      <c r="C39" t="s">
-        <v>78</v>
+      <c r="C39">
+        <v>11.2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>1062292</v>
       </c>
-      <c r="C40" t="s">
-        <v>80</v>
+      <c r="C40">
+        <v>10.3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B41">
         <v>111498</v>
       </c>
-      <c r="C41" t="s">
-        <v>82</v>
+      <c r="C41">
+        <v>12.6</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>372607</v>
       </c>
-      <c r="C42" t="s">
-        <v>84</v>
+      <c r="C42">
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>55927</v>
       </c>
-      <c r="C43" t="s">
-        <v>86</v>
+      <c r="C43">
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>558276</v>
       </c>
-      <c r="C44" t="s">
-        <v>88</v>
+      <c r="C44">
+        <v>10.3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>1854306</v>
       </c>
-      <c r="C45" t="s">
-        <v>90</v>
+      <c r="C45">
+        <v>8.4</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>231080</v>
       </c>
-      <c r="C46" t="s">
-        <v>92</v>
+      <c r="C46">
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>61465</v>
       </c>
-      <c r="C47" t="s">
-        <v>94</v>
+      <c r="C47">
+        <v>11.8</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>661945</v>
       </c>
-      <c r="C48" t="s">
-        <v>96</v>
+      <c r="C48">
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>641131</v>
       </c>
-      <c r="C49" t="s">
-        <v>98</v>
+      <c r="C49">
+        <v>10.5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>171141</v>
       </c>
-      <c r="C50" t="s">
-        <v>100</v>
+      <c r="C50">
+        <v>12.1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>498228</v>
       </c>
-      <c r="C51" t="s">
-        <v>102</v>
+      <c r="C51">
+        <v>10.8</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>43188</v>
       </c>
-      <c r="C52" t="s">
-        <v>104</v>
+      <c r="C52">
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>4997</v>
       </c>
-      <c r="C53" t="s">
-        <v>106</v>
+      <c r="C53">
+        <v>4.7</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>311148</v>
       </c>
-      <c r="C54" t="s">
-        <v>108</v>
+      <c r="C54">
+        <v>11.4</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>3920</v>
       </c>
-      <c r="C55" t="s">
-        <v>110</v>
+      <c r="C55">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>